<commit_message>
Fixed "Swap UART Labels on D0,D1 #7"
Had U0Tx and U0Rx labled incorrectly in schematic.
Fixed labels and rerouted signals to correct pins.
</commit_message>
<xml_diff>
--- a/PinMap.xlsx
+++ b/PinMap.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="11475" windowHeight="4950" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="11475" windowHeight="4950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="245">
   <si>
     <t>Arduino Digital Pins</t>
   </si>
@@ -757,7 +757,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -814,6 +814,22 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -939,7 +955,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -968,24 +984,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -993,17 +1000,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1032,6 +1033,37 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1951,12 +1983,12 @@
       <c r="F37" s="4"/>
     </row>
     <row r="39" spans="4:7">
-      <c r="D39" s="18" t="s">
+      <c r="D39" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
+      <c r="E39" s="44"/>
+      <c r="F39" s="44"/>
+      <c r="G39" s="44"/>
     </row>
     <row r="40" spans="4:7">
       <c r="D40" t="s">
@@ -2461,8 +2493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U44"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="B2" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="40" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="W48" sqref="W48"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="40" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="U43" sqref="U43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2489,7 +2521,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
-      <c r="C1" s="44">
+      <c r="C1" s="39">
         <v>39198</v>
       </c>
       <c r="D1" t="s">
@@ -2497,25 +2529,25 @@
       </c>
     </row>
     <row r="3" spans="1:21">
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="48" t="s">
         <v>120</v>
       </c>
-      <c r="D3" s="23"/>
+      <c r="D3" s="48"/>
     </row>
     <row r="4" spans="1:21">
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="49" t="s">
         <v>119</v>
       </c>
-      <c r="D4" s="24"/>
+      <c r="D4" s="49"/>
     </row>
     <row r="5" spans="1:21">
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="50" t="s">
         <v>242</v>
       </c>
-      <c r="D5" s="25"/>
+      <c r="D5" s="50"/>
     </row>
     <row r="6" spans="1:21">
-      <c r="L6" s="20" t="s">
+      <c r="L6" s="19" t="s">
         <v>239</v>
       </c>
     </row>
@@ -2534,25 +2566,25 @@
       <c r="N8" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="O8" s="38" t="s">
+      <c r="O8" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="33" t="s">
+      <c r="P8" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="Q8" s="33" t="s">
+      <c r="Q8" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="R8" s="33" t="s">
+      <c r="R8" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="S8" s="33" t="s">
+      <c r="S8" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="T8" s="33" t="s">
+      <c r="T8" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="U8" s="33" t="s">
+      <c r="U8" s="28" t="s">
         <v>243</v>
       </c>
     </row>
@@ -2561,37 +2593,37 @@
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
-      <c r="L9" s="34" t="s">
+      <c r="L9" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="M9" s="37" t="s">
+      <c r="M9" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="N9" s="35">
+      <c r="N9" s="30">
         <v>15</v>
       </c>
-      <c r="O9" s="33"/>
-      <c r="P9" s="33"/>
-      <c r="Q9" s="33"/>
-      <c r="R9" s="33"/>
-      <c r="S9" s="33"/>
-      <c r="T9" s="33"/>
-      <c r="U9" s="33"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+      <c r="Q9" s="28"/>
+      <c r="R9" s="28"/>
+      <c r="S9" s="28"/>
+      <c r="T9" s="28"/>
+      <c r="U9" s="28"/>
     </row>
     <row r="10" spans="1:21">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="C10" s="33" t="s">
+      <c r="C10" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="D10" s="33" t="s">
+      <c r="D10" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="E10" s="45" t="s">
+      <c r="E10" s="40" t="s">
         <v>7</v>
       </c>
       <c r="F10" s="13" t="s">
@@ -2600,13 +2632,13 @@
       <c r="G10" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="L10" s="30" t="s">
+      <c r="L10" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="M10" s="41" t="s">
+      <c r="M10" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="N10" s="31">
+      <c r="N10" s="27">
         <v>14</v>
       </c>
       <c r="O10" s="5"/>
@@ -2618,23 +2650,23 @@
       <c r="U10" s="5"/>
     </row>
     <row r="11" spans="1:21">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="28" t="s">
         <v>185</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33" t="s">
+      <c r="B11" s="28"/>
+      <c r="C11" s="28" t="s">
         <v>183</v>
       </c>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="35">
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="30">
         <v>35</v>
       </c>
-      <c r="G11" s="33"/>
-      <c r="H11" s="34" t="s">
+      <c r="G11" s="28"/>
+      <c r="H11" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="L11" s="39" t="s">
+      <c r="L11" s="34" t="s">
         <v>241</v>
       </c>
       <c r="M11" s="7"/>
@@ -2656,14 +2688,14 @@
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="31">
+      <c r="F12" s="27">
         <v>36</v>
       </c>
       <c r="G12" s="5"/>
-      <c r="H12" s="30" t="s">
+      <c r="H12" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="L12" s="40" t="s">
+      <c r="L12" s="35" t="s">
         <v>237</v>
       </c>
       <c r="M12" s="7"/>
@@ -2676,33 +2708,33 @@
       <c r="T12" s="7"/>
     </row>
     <row r="13" spans="1:21">
-      <c r="H13" s="22"/>
-      <c r="L13" s="34" t="s">
+      <c r="H13" s="21"/>
+      <c r="L13" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="M13" s="33"/>
-      <c r="N13" s="35">
+      <c r="M13" s="28"/>
+      <c r="N13" s="30">
         <v>13</v>
       </c>
-      <c r="O13" s="33"/>
-      <c r="P13" s="33"/>
-      <c r="Q13" s="33" t="s">
+      <c r="O13" s="28"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="R13" s="33"/>
-      <c r="S13" s="33" t="s">
+      <c r="R13" s="28"/>
+      <c r="S13" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="T13" s="33"/>
-      <c r="U13" s="33"/>
+      <c r="T13" s="28"/>
+      <c r="U13" s="28"/>
     </row>
     <row r="14" spans="1:21">
-      <c r="H14" s="22"/>
-      <c r="L14" s="27" t="s">
+      <c r="H14" s="21"/>
+      <c r="L14" s="24" t="s">
         <v>33</v>
       </c>
       <c r="M14" s="7"/>
-      <c r="N14" s="28">
+      <c r="N14" s="25">
         <v>12</v>
       </c>
       <c r="O14" s="7"/>
@@ -2724,14 +2756,14 @@
       </c>
     </row>
     <row r="15" spans="1:21">
-      <c r="H15" s="21" t="s">
+      <c r="H15" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="L15" s="27" t="s">
+      <c r="L15" s="24" t="s">
         <v>36</v>
       </c>
       <c r="M15" s="7"/>
-      <c r="N15" s="28">
+      <c r="N15" s="25">
         <v>11</v>
       </c>
       <c r="O15" s="7"/>
@@ -2749,14 +2781,14 @@
       <c r="U15" s="7"/>
     </row>
     <row r="16" spans="1:21">
-      <c r="H16" s="20" t="s">
+      <c r="H16" s="19" t="s">
         <v>238</v>
       </c>
-      <c r="L16" s="27" t="s">
+      <c r="L16" s="24" t="s">
         <v>34</v>
       </c>
       <c r="M16" s="7"/>
-      <c r="N16" s="28">
+      <c r="N16" s="25">
         <v>10</v>
       </c>
       <c r="O16" s="7"/>
@@ -2774,16 +2806,16 @@
       <c r="U16" s="7"/>
     </row>
     <row r="17" spans="1:21">
-      <c r="H17" s="20" t="s">
+      <c r="H17" s="19" t="s">
         <v>239</v>
       </c>
-      <c r="L17" s="27" t="s">
+      <c r="L17" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="M17" s="36" t="s">
+      <c r="M17" s="31" t="s">
         <v>182</v>
       </c>
-      <c r="N17" s="28">
+      <c r="N17" s="25">
         <v>9</v>
       </c>
       <c r="O17" s="7" t="s">
@@ -2804,16 +2836,16 @@
     </row>
     <row r="18" spans="1:21">
       <c r="F18" s="7"/>
-      <c r="H18" s="19" t="s">
+      <c r="H18" s="18" t="s">
         <v>237</v>
       </c>
-      <c r="L18" s="30" t="s">
+      <c r="L18" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="M18" s="41" t="s">
+      <c r="M18" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="N18" s="31">
+      <c r="N18" s="27">
         <v>8</v>
       </c>
       <c r="O18" s="5" t="s">
@@ -2834,46 +2866,46 @@
     </row>
     <row r="19" spans="1:21">
       <c r="F19" s="7"/>
-      <c r="H19" s="19" t="s">
+      <c r="H19" s="18" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="20" spans="1:21">
-      <c r="L20" s="34" t="s">
+      <c r="L20" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="M20" s="37" t="s">
+      <c r="M20" s="32" t="s">
         <v>180</v>
       </c>
-      <c r="N20" s="35">
+      <c r="N20" s="30">
         <v>7</v>
       </c>
-      <c r="O20" s="33" t="s">
+      <c r="O20" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="P20" s="33"/>
-      <c r="Q20" s="33" t="s">
+      <c r="P20" s="28"/>
+      <c r="Q20" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="R20" s="33"/>
-      <c r="S20" s="33" t="s">
+      <c r="R20" s="28"/>
+      <c r="S20" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="T20" s="33" t="s">
+      <c r="T20" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="U20" s="33"/>
+      <c r="U20" s="28"/>
     </row>
     <row r="21" spans="1:21">
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-      <c r="L21" s="27" t="s">
+      <c r="L21" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="M21" s="36" t="s">
+      <c r="M21" s="31" t="s">
         <v>179</v>
       </c>
-      <c r="N21" s="28">
+      <c r="N21" s="25">
         <v>6</v>
       </c>
       <c r="O21" s="7" t="s">
@@ -2893,29 +2925,29 @@
       <c r="U21" s="7"/>
     </row>
     <row r="22" spans="1:21">
-      <c r="A22" s="33"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33" t="s">
+      <c r="A22" s="28"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="F22" s="35">
+      <c r="F22" s="30">
         <v>16</v>
       </c>
-      <c r="G22" s="37" t="s">
+      <c r="G22" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="H22" s="34" t="s">
+      <c r="H22" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="L22" s="27" t="s">
+      <c r="L22" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="M22" s="36" t="s">
+      <c r="M22" s="31" t="s">
         <v>178</v>
       </c>
-      <c r="N22" s="28">
+      <c r="N22" s="25">
         <v>5</v>
       </c>
       <c r="O22" s="7" t="s">
@@ -2944,22 +2976,22 @@
       <c r="E23" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F23" s="28">
+      <c r="F23" s="25">
         <v>17</v>
       </c>
-      <c r="G23" s="36" t="s">
+      <c r="G23" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="H23" s="27" t="s">
+      <c r="H23" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="L23" s="27" t="s">
+      <c r="L23" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="M23" s="36" t="s">
+      <c r="M23" s="31" t="s">
         <v>177</v>
       </c>
-      <c r="N23" s="28">
+      <c r="N23" s="25">
         <v>4</v>
       </c>
       <c r="O23" s="7" t="s">
@@ -2990,20 +3022,20 @@
       <c r="E24" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="F24" s="28">
+      <c r="F24" s="25">
         <v>18</v>
       </c>
-      <c r="G24" s="36" t="s">
+      <c r="G24" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="H24" s="27" t="s">
+      <c r="H24" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="L24" s="27" t="s">
+      <c r="L24" s="24" t="s">
         <v>17</v>
       </c>
       <c r="M24" s="7"/>
-      <c r="N24" s="28">
+      <c r="N24" s="25">
         <v>3</v>
       </c>
       <c r="O24" s="7"/>
@@ -3028,20 +3060,20 @@
       <c r="E25" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="F25" s="28">
+      <c r="F25" s="25">
         <v>19</v>
       </c>
-      <c r="G25" s="36" t="s">
+      <c r="G25" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="H25" s="27" t="s">
+      <c r="H25" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="L25" s="27" t="s">
+      <c r="L25" s="24" t="s">
         <v>18</v>
       </c>
       <c r="M25" s="7"/>
-      <c r="N25" s="28">
+      <c r="N25" s="25">
         <v>2</v>
       </c>
       <c r="O25" s="7"/>
@@ -3062,20 +3094,20 @@
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
-      <c r="F26" s="28">
+      <c r="F26" s="25">
         <v>20</v>
       </c>
-      <c r="G26" s="36" t="s">
+      <c r="G26" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="H26" s="27" t="s">
+      <c r="H26" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="L26" s="27" t="s">
+      <c r="L26" s="24" t="s">
         <v>9</v>
       </c>
       <c r="M26" s="7"/>
-      <c r="N26" s="28">
+      <c r="N26" s="25">
         <v>1</v>
       </c>
       <c r="O26" s="7"/>
@@ -3096,20 +3128,20 @@
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
-      <c r="F27" s="31">
+      <c r="F27" s="27">
         <v>21</v>
       </c>
-      <c r="G27" s="41" t="s">
+      <c r="G27" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="H27" s="30" t="s">
+      <c r="H27" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="L27" s="30" t="s">
+      <c r="L27" s="26" t="s">
         <v>11</v>
       </c>
       <c r="M27" s="5"/>
-      <c r="N27" s="31">
+      <c r="N27" s="27">
         <v>0</v>
       </c>
       <c r="O27" s="5"/>
@@ -3135,63 +3167,63 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="N31" s="1"/>
-      <c r="O31" s="38" t="s">
+      <c r="O31" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="P31" s="33" t="s">
+      <c r="P31" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="Q31" s="33" t="s">
+      <c r="Q31" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="R31" s="33" t="s">
+      <c r="R31" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="S31" s="33" t="s">
+      <c r="S31" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="T31" s="33" t="s">
+      <c r="T31" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="U31" s="33" t="s">
+      <c r="U31" s="28" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="32" spans="1:21">
-      <c r="A32" s="33"/>
-      <c r="B32" s="33"/>
-      <c r="C32" s="33" t="s">
+      <c r="A32" s="28"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33" t="s">
+      <c r="D32" s="28"/>
+      <c r="E32" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="F32" s="35">
+      <c r="F32" s="30">
         <v>20</v>
       </c>
-      <c r="G32" s="37" t="s">
+      <c r="G32" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="H32" s="34" t="s">
+      <c r="H32" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="L32" s="34" t="s">
+      <c r="L32" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="M32" s="33"/>
-      <c r="N32" s="35">
+      <c r="M32" s="28"/>
+      <c r="N32" s="30">
         <v>22</v>
       </c>
-      <c r="O32" s="33"/>
-      <c r="P32" s="33" t="s">
+      <c r="O32" s="28"/>
+      <c r="P32" s="28" t="s">
         <v>156</v>
       </c>
-      <c r="Q32" s="33"/>
-      <c r="R32" s="33"/>
-      <c r="S32" s="33"/>
-      <c r="T32" s="33"/>
-      <c r="U32" s="33" t="s">
+      <c r="Q32" s="28"/>
+      <c r="R32" s="28"/>
+      <c r="S32" s="28"/>
+      <c r="T32" s="28"/>
+      <c r="U32" s="28" t="s">
         <v>165</v>
       </c>
     </row>
@@ -3205,20 +3237,20 @@
       <c r="E33" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="F33" s="31">
+      <c r="F33" s="27">
         <v>21</v>
       </c>
-      <c r="G33" s="41" t="s">
+      <c r="G33" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="H33" s="30" t="s">
+      <c r="H33" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="L33" s="27" t="s">
+      <c r="L33" s="24" t="s">
         <v>102</v>
       </c>
       <c r="M33" s="7"/>
-      <c r="N33" s="28">
+      <c r="N33" s="25">
         <v>23</v>
       </c>
       <c r="O33" s="7"/>
@@ -3234,27 +3266,27 @@
       </c>
     </row>
     <row r="34" spans="1:21">
-      <c r="A34" s="33"/>
-      <c r="B34" s="33" t="s">
+      <c r="A34" s="28"/>
+      <c r="B34" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="35">
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="30">
         <v>14</v>
       </c>
-      <c r="G34" s="37" t="s">
+      <c r="G34" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="H34" s="34" t="s">
+      <c r="H34" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="L34" s="27" t="s">
+      <c r="L34" s="24" t="s">
         <v>101</v>
       </c>
       <c r="M34" s="7"/>
-      <c r="N34" s="28">
+      <c r="N34" s="25">
         <v>24</v>
       </c>
       <c r="O34" s="7"/>
@@ -3279,20 +3311,20 @@
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
-      <c r="F35" s="31">
+      <c r="F35" s="27">
         <v>15</v>
       </c>
-      <c r="G35" s="41" t="s">
+      <c r="G35" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="H35" s="30" t="s">
+      <c r="H35" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="L35" s="30" t="s">
+      <c r="L35" s="26" t="s">
         <v>100</v>
       </c>
       <c r="M35" s="5"/>
-      <c r="N35" s="31">
+      <c r="N35" s="27">
         <v>25</v>
       </c>
       <c r="O35" s="5"/>
@@ -3310,35 +3342,35 @@
       </c>
     </row>
     <row r="36" spans="1:21">
-      <c r="J36" s="32" t="s">
+      <c r="J36" s="45" t="s">
         <v>188</v>
       </c>
-      <c r="K36" s="33"/>
-      <c r="L36" s="27" t="s">
+      <c r="K36" s="28"/>
+      <c r="L36" s="24" t="s">
         <v>57</v>
       </c>
       <c r="M36" s="7"/>
-      <c r="N36" s="35">
+      <c r="N36" s="30">
         <v>26</v>
       </c>
-      <c r="O36" s="33"/>
-      <c r="P36" s="33"/>
-      <c r="Q36" s="33" t="s">
+      <c r="O36" s="28"/>
+      <c r="P36" s="28"/>
+      <c r="Q36" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="R36" s="33"/>
-      <c r="S36" s="33"/>
-      <c r="T36" s="33"/>
-      <c r="U36" s="33"/>
+      <c r="R36" s="28"/>
+      <c r="S36" s="28"/>
+      <c r="T36" s="28"/>
+      <c r="U36" s="28"/>
     </row>
     <row r="37" spans="1:21">
-      <c r="J37" s="26"/>
+      <c r="J37" s="46"/>
       <c r="K37" s="7"/>
-      <c r="L37" s="27" t="s">
+      <c r="L37" s="24" t="s">
         <v>58</v>
       </c>
       <c r="M37" s="7"/>
-      <c r="N37" s="28">
+      <c r="N37" s="25">
         <v>27</v>
       </c>
       <c r="O37" s="7"/>
@@ -3352,13 +3384,13 @@
       <c r="U37" s="7"/>
     </row>
     <row r="38" spans="1:21">
-      <c r="J38" s="26"/>
+      <c r="J38" s="46"/>
       <c r="K38" s="7"/>
-      <c r="L38" s="27" t="s">
+      <c r="L38" s="24" t="s">
         <v>59</v>
       </c>
       <c r="M38" s="7"/>
-      <c r="N38" s="28">
+      <c r="N38" s="25">
         <v>28</v>
       </c>
       <c r="O38" s="7"/>
@@ -3372,13 +3404,13 @@
       <c r="U38" s="7"/>
     </row>
     <row r="39" spans="1:21">
-      <c r="J39" s="29"/>
+      <c r="J39" s="47"/>
       <c r="K39" s="5"/>
-      <c r="L39" s="30" t="s">
+      <c r="L39" s="26" t="s">
         <v>60</v>
       </c>
       <c r="M39" s="5"/>
-      <c r="N39" s="31">
+      <c r="N39" s="27">
         <v>29</v>
       </c>
       <c r="O39" s="5"/>
@@ -3392,41 +3424,41 @@
       <c r="U39" s="5"/>
     </row>
     <row r="40" spans="1:21">
-      <c r="J40" s="32" t="s">
+      <c r="J40" s="45" t="s">
         <v>187</v>
       </c>
-      <c r="K40" s="33" t="s">
+      <c r="K40" s="28" t="s">
         <v>168</v>
       </c>
-      <c r="L40" s="34" t="s">
+      <c r="L40" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="M40" s="33"/>
-      <c r="N40" s="35">
+      <c r="M40" s="28"/>
+      <c r="N40" s="30">
         <v>30</v>
       </c>
-      <c r="O40" s="33"/>
-      <c r="P40" s="33" t="s">
+      <c r="O40" s="28"/>
+      <c r="P40" s="28" t="s">
         <v>172</v>
       </c>
-      <c r="Q40" s="33"/>
-      <c r="R40" s="33"/>
-      <c r="S40" s="33"/>
-      <c r="T40" s="33"/>
-      <c r="U40" s="33" t="s">
+      <c r="Q40" s="28"/>
+      <c r="R40" s="28"/>
+      <c r="S40" s="28"/>
+      <c r="T40" s="28"/>
+      <c r="U40" s="28" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="41" spans="1:21">
-      <c r="J41" s="26"/>
+      <c r="J41" s="46"/>
       <c r="K41" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="L41" s="27" t="s">
+      <c r="L41" s="24" t="s">
         <v>88</v>
       </c>
       <c r="M41" s="7"/>
-      <c r="N41" s="28">
+      <c r="N41" s="25">
         <v>31</v>
       </c>
       <c r="O41" s="7"/>
@@ -3442,15 +3474,15 @@
       </c>
     </row>
     <row r="42" spans="1:21">
-      <c r="J42" s="26"/>
+      <c r="J42" s="46"/>
       <c r="K42" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="L42" s="27" t="s">
+      <c r="L42" s="24" t="s">
         <v>106</v>
       </c>
       <c r="M42" s="7"/>
-      <c r="N42" s="28">
+      <c r="N42" s="25">
         <v>32</v>
       </c>
       <c r="O42" s="7"/>
@@ -3464,15 +3496,15 @@
       <c r="U42" s="7"/>
     </row>
     <row r="43" spans="1:21">
-      <c r="J43" s="29"/>
+      <c r="J43" s="47"/>
       <c r="K43" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="L43" s="30" t="s">
+      <c r="L43" s="26" t="s">
         <v>107</v>
       </c>
       <c r="M43" s="5"/>
-      <c r="N43" s="31">
+      <c r="N43" s="27">
         <v>33</v>
       </c>
       <c r="O43" s="5"/>
@@ -3488,11 +3520,11 @@
       </c>
     </row>
     <row r="44" spans="1:21">
-      <c r="L44" s="42" t="s">
+      <c r="L44" s="37" t="s">
         <v>108</v>
       </c>
       <c r="M44" s="8"/>
-      <c r="N44" s="43">
+      <c r="N44" s="38">
         <v>34</v>
       </c>
       <c r="O44" s="8"/>
@@ -3524,13 +3556,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:M44"/>
+  <dimension ref="B2:M88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:N45"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:13">
       <c r="B2" s="14" t="s">
@@ -3583,27 +3619,27 @@
         <v>198</v>
       </c>
       <c r="F4" t="str">
-        <f>CONCATENATE(LEFT(B4,2),"_",RIGHT(B4,1))</f>
+        <f t="shared" ref="F4:F40" si="0">CONCATENATE(LEFT(B4,2),"_",RIGHT(B4,1))</f>
         <v>PA_1</v>
       </c>
       <c r="H4" t="str">
-        <f>CONCATENATE("static const uint8_t ",F4," = ", C4,";")</f>
+        <f t="shared" ref="H4:H44" si="1">CONCATENATE("static const uint8_t ",F4," = ", C4,";")</f>
         <v>static const uint8_t PA_1 = 0;</v>
       </c>
       <c r="J4" t="str">
-        <f>CONCATENATE(D4,", /* ", C4," - ",F4," */")</f>
+        <f t="shared" ref="J4:J40" si="2">CONCATENATE(D4,", /* ", C4," - ",F4," */")</f>
         <v>NOT_ON_TIMER, /* 0 - PA_1 */</v>
       </c>
       <c r="K4" t="str">
-        <f>CONCATENATE(LEFT(B4,2), ", /* ", C4," - ",F4, " */")</f>
+        <f t="shared" ref="K4:K40" si="3">CONCATENATE(LEFT(B4,2), ", /* ", C4," - ",F4, " */")</f>
         <v>PA, /* 0 - PA_1 */</v>
       </c>
       <c r="L4" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B4,1),"),"," /* ",C4," - ",F4," */")</f>
+        <f t="shared" ref="L4:L40" si="4">CONCATENATE("BV(",RIGHT(B4,1),"),"," /* ",C4," - ",F4," */")</f>
         <v>BV(1), /* 0 - PA_1 */</v>
       </c>
       <c r="M4" t="str">
-        <f>IF(ISBLANK(E4),CONCATENATE("NOT_ON_ADC", ", /* ", C4," - ",F4, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E4,LEN(E4)-1), ", /* ", C4," - ",F4, " */"))</f>
+        <f t="shared" ref="M4:M40" si="5">IF(ISBLANK(E4),CONCATENATE("NOT_ON_ADC", ", /* ", C4," - ",F4, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E4,LEN(E4)-1), ", /* ", C4," - ",F4, " */"))</f>
         <v>NOT_ON_ADC, /* 0 - PA_1 */</v>
       </c>
     </row>
@@ -3618,27 +3654,27 @@
         <v>198</v>
       </c>
       <c r="F5" t="str">
-        <f>CONCATENATE(LEFT(B5,2),"_",RIGHT(B5,1))</f>
+        <f t="shared" si="0"/>
         <v>PA_0</v>
       </c>
       <c r="H5" t="str">
-        <f>CONCATENATE("static const uint8_t ",F5," = ", C5,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PA_0 = 1;</v>
       </c>
       <c r="J5" t="str">
-        <f>CONCATENATE(D5,", /* ", C5," - ",F5," */")</f>
+        <f t="shared" si="2"/>
         <v>NOT_ON_TIMER, /* 1 - PA_0 */</v>
       </c>
       <c r="K5" t="str">
-        <f>CONCATENATE(LEFT(B5,2), ", /* ", C5," - ",F5, " */")</f>
+        <f t="shared" si="3"/>
         <v>PA, /* 1 - PA_0 */</v>
       </c>
       <c r="L5" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B5,1),"),"," /* ",C5," - ",F5," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(0), /* 1 - PA_0 */</v>
       </c>
       <c r="M5" t="str">
-        <f>IF(ISBLANK(E5),CONCATENATE("NOT_ON_ADC", ", /* ", C5," - ",F5, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E5,LEN(E5)-1), ", /* ", C5," - ",F5, " */"))</f>
+        <f t="shared" si="5"/>
         <v>NOT_ON_ADC, /* 1 - PA_0 */</v>
       </c>
     </row>
@@ -3653,27 +3689,27 @@
         <v>198</v>
       </c>
       <c r="F6" t="str">
-        <f>CONCATENATE(LEFT(B6,2),"_",RIGHT(B6,1))</f>
+        <f t="shared" si="0"/>
         <v>PA_7</v>
       </c>
       <c r="H6" t="str">
-        <f>CONCATENATE("static const uint8_t ",F6," = ", C6,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PA_7 = 2;</v>
       </c>
       <c r="J6" t="str">
-        <f>CONCATENATE(D6,", /* ", C6," - ",F6," */")</f>
+        <f t="shared" si="2"/>
         <v>NOT_ON_TIMER, /* 2 - PA_7 */</v>
       </c>
       <c r="K6" t="str">
-        <f>CONCATENATE(LEFT(B6,2), ", /* ", C6," - ",F6, " */")</f>
+        <f t="shared" si="3"/>
         <v>PA, /* 2 - PA_7 */</v>
       </c>
       <c r="L6" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B6,1),"),"," /* ",C6," - ",F6," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(7), /* 2 - PA_7 */</v>
       </c>
       <c r="M6" t="str">
-        <f>IF(ISBLANK(E6),CONCATENATE("NOT_ON_ADC", ", /* ", C6," - ",F6, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E6,LEN(E6)-1), ", /* ", C6," - ",F6, " */"))</f>
+        <f t="shared" si="5"/>
         <v>NOT_ON_ADC, /* 2 - PA_7 */</v>
       </c>
     </row>
@@ -3688,27 +3724,27 @@
         <v>198</v>
       </c>
       <c r="F7" t="str">
-        <f>CONCATENATE(LEFT(B7,2),"_",RIGHT(B7,1))</f>
+        <f t="shared" si="0"/>
         <v>PA_6</v>
       </c>
       <c r="H7" t="str">
-        <f>CONCATENATE("static const uint8_t ",F7," = ", C7,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PA_6 = 3;</v>
       </c>
       <c r="J7" t="str">
-        <f>CONCATENATE(D7,", /* ", C7," - ",F7," */")</f>
+        <f t="shared" si="2"/>
         <v>NOT_ON_TIMER, /* 3 - PA_6 */</v>
       </c>
       <c r="K7" t="str">
-        <f>CONCATENATE(LEFT(B7,2), ", /* ", C7," - ",F7, " */")</f>
+        <f t="shared" si="3"/>
         <v>PA, /* 3 - PA_6 */</v>
       </c>
       <c r="L7" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B7,1),"),"," /* ",C7," - ",F7," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(6), /* 3 - PA_6 */</v>
       </c>
       <c r="M7" t="str">
-        <f>IF(ISBLANK(E7),CONCATENATE("NOT_ON_ADC", ", /* ", C7," - ",F7, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E7,LEN(E7)-1), ", /* ", C7," - ",F7, " */"))</f>
+        <f t="shared" si="5"/>
         <v>NOT_ON_ADC, /* 3 - PA_6 */</v>
       </c>
     </row>
@@ -3726,31 +3762,31 @@
         <v>177</v>
       </c>
       <c r="F8" t="str">
-        <f>CONCATENATE(LEFT(B8,2),"_",RIGHT(B8,1))</f>
+        <f t="shared" si="0"/>
         <v>PE_4</v>
       </c>
       <c r="H8" t="str">
-        <f>CONCATENATE("static const uint8_t ",F8," = ", C8,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PE_4 = 4;</v>
       </c>
       <c r="I8" t="str">
-        <f>CONCATENATE("static const uint8_t ",E8," = ", C8,"; // ",F8)</f>
+        <f t="shared" ref="I8:I13" si="6">CONCATENATE("static const uint8_t ",E8," = ", C8,"; // ",F8)</f>
         <v>static const uint8_t A6 = 4; // PE_4</v>
       </c>
       <c r="J8" t="str">
-        <f>CONCATENATE(D8,", /* ", C8," - ",F8," */")</f>
+        <f t="shared" si="2"/>
         <v>NOT_ON_TIMER, /* 4 - PE_4 */</v>
       </c>
       <c r="K8" t="str">
-        <f>CONCATENATE(LEFT(B8,2), ", /* ", C8," - ",F8, " */")</f>
+        <f t="shared" si="3"/>
         <v>PE, /* 4 - PE_4 */</v>
       </c>
       <c r="L8" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B8,1),"),"," /* ",C8," - ",F8," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(4), /* 4 - PE_4 */</v>
       </c>
       <c r="M8" t="str">
-        <f>IF(ISBLANK(E8),CONCATENATE("NOT_ON_ADC", ", /* ", C8," - ",F8, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E8,LEN(E8)-1), ", /* ", C8," - ",F8, " */"))</f>
+        <f t="shared" si="5"/>
         <v>ADC_CTL_CH6, /* 4 - PE_4 */</v>
       </c>
     </row>
@@ -3768,31 +3804,31 @@
         <v>178</v>
       </c>
       <c r="F9" t="str">
-        <f>CONCATENATE(LEFT(B9,2),"_",RIGHT(B9,1))</f>
+        <f t="shared" si="0"/>
         <v>PE_5</v>
       </c>
       <c r="H9" t="str">
-        <f>CONCATENATE("static const uint8_t ",F9," = ", C9,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PE_5 = 5;</v>
       </c>
       <c r="I9" t="str">
-        <f>CONCATENATE("static const uint8_t ",E9," = ", C9,"; // ",F9)</f>
+        <f t="shared" si="6"/>
         <v>static const uint8_t A7 = 5; // PE_5</v>
       </c>
       <c r="J9" t="str">
-        <f>CONCATENATE(D9,", /* ", C9," - ",F9," */")</f>
+        <f t="shared" si="2"/>
         <v>NOT_ON_TIMER, /* 5 - PE_5 */</v>
       </c>
       <c r="K9" t="str">
-        <f>CONCATENATE(LEFT(B9,2), ", /* ", C9," - ",F9, " */")</f>
+        <f t="shared" si="3"/>
         <v>PE, /* 5 - PE_5 */</v>
       </c>
       <c r="L9" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B9,1),"),"," /* ",C9," - ",F9," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(5), /* 5 - PE_5 */</v>
       </c>
       <c r="M9" t="str">
-        <f>IF(ISBLANK(E9),CONCATENATE("NOT_ON_ADC", ", /* ", C9," - ",F9, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E9,LEN(E9)-1), ", /* ", C9," - ",F9, " */"))</f>
+        <f t="shared" si="5"/>
         <v>ADC_CTL_CH7, /* 5 - PE_5 */</v>
       </c>
     </row>
@@ -3810,31 +3846,31 @@
         <v>179</v>
       </c>
       <c r="F10" t="str">
-        <f>CONCATENATE(LEFT(B10,2),"_",RIGHT(B10,1))</f>
+        <f t="shared" si="0"/>
         <v>PB_4</v>
       </c>
       <c r="H10" t="str">
-        <f>CONCATENATE("static const uint8_t ",F10," = ", C10,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PB_4 = 6;</v>
       </c>
       <c r="I10" t="str">
-        <f>CONCATENATE("static const uint8_t ",E10," = ", C10,"; // ",F10)</f>
+        <f t="shared" si="6"/>
         <v>static const uint8_t A8 = 6; // PB_4</v>
       </c>
       <c r="J10" t="str">
-        <f>CONCATENATE(D10,", /* ", C10," - ",F10," */")</f>
+        <f t="shared" si="2"/>
         <v>T1A0, /* 6 - PB_4 */</v>
       </c>
       <c r="K10" t="str">
-        <f>CONCATENATE(LEFT(B10,2), ", /* ", C10," - ",F10, " */")</f>
+        <f t="shared" si="3"/>
         <v>PB, /* 6 - PB_4 */</v>
       </c>
       <c r="L10" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B10,1),"),"," /* ",C10," - ",F10," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(4), /* 6 - PB_4 */</v>
       </c>
       <c r="M10" t="str">
-        <f>IF(ISBLANK(E10),CONCATENATE("NOT_ON_ADC", ", /* ", C10," - ",F10, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E10,LEN(E10)-1), ", /* ", C10," - ",F10, " */"))</f>
+        <f t="shared" si="5"/>
         <v>ADC_CTL_CH8, /* 6 - PB_4 */</v>
       </c>
     </row>
@@ -3852,31 +3888,31 @@
         <v>180</v>
       </c>
       <c r="F11" t="str">
-        <f>CONCATENATE(LEFT(B11,2),"_",RIGHT(B11,1))</f>
+        <f t="shared" si="0"/>
         <v>PB_5</v>
       </c>
       <c r="H11" t="str">
-        <f>CONCATENATE("static const uint8_t ",F11," = ", C11,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PB_5 = 7;</v>
       </c>
       <c r="I11" t="str">
-        <f>CONCATENATE("static const uint8_t ",E11," = ", C11,"; // ",F11)</f>
+        <f t="shared" si="6"/>
         <v>static const uint8_t A9 = 7; // PB_5</v>
       </c>
       <c r="J11" t="str">
-        <f>CONCATENATE(D11,", /* ", C11," - ",F11," */")</f>
+        <f t="shared" si="2"/>
         <v>T1B0, /* 7 - PB_5 */</v>
       </c>
       <c r="K11" t="str">
-        <f>CONCATENATE(LEFT(B11,2), ", /* ", C11," - ",F11, " */")</f>
+        <f t="shared" si="3"/>
         <v>PB, /* 7 - PB_5 */</v>
       </c>
       <c r="L11" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B11,1),"),"," /* ",C11," - ",F11," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(5), /* 7 - PB_5 */</v>
       </c>
       <c r="M11" t="str">
-        <f>IF(ISBLANK(E11),CONCATENATE("NOT_ON_ADC", ", /* ", C11," - ",F11, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E11,LEN(E11)-1), ", /* ", C11," - ",F11, " */"))</f>
+        <f t="shared" si="5"/>
         <v>ADC_CTL_CH9, /* 7 - PB_5 */</v>
       </c>
     </row>
@@ -3894,31 +3930,31 @@
         <v>181</v>
       </c>
       <c r="F12" t="str">
-        <f>CONCATENATE(LEFT(B12,2),"_",RIGHT(B12,1))</f>
+        <f t="shared" si="0"/>
         <v>PD_1</v>
       </c>
       <c r="H12" t="str">
-        <f>CONCATENATE("static const uint8_t ",F12," = ", C12,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PD_1 = 8;</v>
       </c>
       <c r="I12" t="str">
-        <f>CONCATENATE("static const uint8_t ",E12," = ", C12,"; // ",F12)</f>
+        <f t="shared" si="6"/>
         <v>static const uint8_t A10 = 8; // PD_1</v>
       </c>
       <c r="J12" t="str">
-        <f>CONCATENATE(D12,", /* ", C12," - ",F12," */")</f>
+        <f t="shared" si="2"/>
         <v>WT2B, /* 8 - PD_1 */</v>
       </c>
       <c r="K12" t="str">
-        <f>CONCATENATE(LEFT(B12,2), ", /* ", C12," - ",F12, " */")</f>
+        <f t="shared" si="3"/>
         <v>PD, /* 8 - PD_1 */</v>
       </c>
       <c r="L12" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B12,1),"),"," /* ",C12," - ",F12," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(1), /* 8 - PD_1 */</v>
       </c>
       <c r="M12" t="str">
-        <f>IF(ISBLANK(E12),CONCATENATE("NOT_ON_ADC", ", /* ", C12," - ",F12, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E12,LEN(E12)-1), ", /* ", C12," - ",F12, " */"))</f>
+        <f t="shared" si="5"/>
         <v>ADC_CTL_CH10, /* 8 - PD_1 */</v>
       </c>
     </row>
@@ -3936,31 +3972,31 @@
         <v>182</v>
       </c>
       <c r="F13" t="str">
-        <f>CONCATENATE(LEFT(B13,2),"_",RIGHT(B13,1))</f>
+        <f t="shared" si="0"/>
         <v>PD_0</v>
       </c>
       <c r="H13" t="str">
-        <f>CONCATENATE("static const uint8_t ",F13," = ", C13,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PD_0 = 9;</v>
       </c>
       <c r="I13" t="str">
-        <f>CONCATENATE("static const uint8_t ",E13," = ", C13,"; // ",F13)</f>
+        <f t="shared" si="6"/>
         <v>static const uint8_t A11 = 9; // PD_0</v>
       </c>
       <c r="J13" t="str">
-        <f>CONCATENATE(D13,", /* ", C13," - ",F13," */")</f>
+        <f t="shared" si="2"/>
         <v>WT2A, /* 9 - PD_0 */</v>
       </c>
       <c r="K13" t="str">
-        <f>CONCATENATE(LEFT(B13,2), ", /* ", C13," - ",F13, " */")</f>
+        <f t="shared" si="3"/>
         <v>PD, /* 9 - PD_0 */</v>
       </c>
       <c r="L13" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B13,1),"),"," /* ",C13," - ",F13," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(0), /* 9 - PD_0 */</v>
       </c>
       <c r="M13" t="str">
-        <f>IF(ISBLANK(E13),CONCATENATE("NOT_ON_ADC", ", /* ", C13," - ",F13, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E13,LEN(E13)-1), ", /* ", C13," - ",F13, " */"))</f>
+        <f t="shared" si="5"/>
         <v>ADC_CTL_CH11, /* 9 - PD_0 */</v>
       </c>
     </row>
@@ -3975,27 +4011,27 @@
         <v>217</v>
       </c>
       <c r="F14" t="str">
-        <f>CONCATENATE(LEFT(B14,2),"_",RIGHT(B14,1))</f>
+        <f t="shared" si="0"/>
         <v>PF_3</v>
       </c>
       <c r="H14" t="str">
-        <f>CONCATENATE("static const uint8_t ",F14," = ", C14,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PF_3 = 10;</v>
       </c>
       <c r="J14" t="str">
-        <f>CONCATENATE(D14,", /* ", C14," - ",F14," */")</f>
+        <f t="shared" si="2"/>
         <v>T1B1, /* 10 - PF_3 */</v>
       </c>
       <c r="K14" t="str">
-        <f>CONCATENATE(LEFT(B14,2), ", /* ", C14," - ",F14, " */")</f>
+        <f t="shared" si="3"/>
         <v>PF, /* 10 - PF_3 */</v>
       </c>
       <c r="L14" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B14,1),"),"," /* ",C14," - ",F14," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(3), /* 10 - PF_3 */</v>
       </c>
       <c r="M14" t="str">
-        <f>IF(ISBLANK(E14),CONCATENATE("NOT_ON_ADC", ", /* ", C14," - ",F14, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E14,LEN(E14)-1), ", /* ", C14," - ",F14, " */"))</f>
+        <f t="shared" si="5"/>
         <v>NOT_ON_ADC, /* 10 - PF_3 */</v>
       </c>
     </row>
@@ -4010,62 +4046,62 @@
         <v>208</v>
       </c>
       <c r="F15" t="str">
-        <f>CONCATENATE(LEFT(B15,2),"_",RIGHT(B15,1))</f>
+        <f t="shared" si="0"/>
         <v>PF_1</v>
       </c>
       <c r="H15" t="str">
-        <f>CONCATENATE("static const uint8_t ",F15," = ", C15,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PF_1 = 11;</v>
       </c>
       <c r="J15" t="str">
-        <f>CONCATENATE(D15,", /* ", C15," - ",F15," */")</f>
+        <f t="shared" si="2"/>
         <v>T0B1, /* 11 - PF_1 */</v>
       </c>
       <c r="K15" t="str">
-        <f>CONCATENATE(LEFT(B15,2), ", /* ", C15," - ",F15, " */")</f>
+        <f t="shared" si="3"/>
         <v>PF, /* 11 - PF_1 */</v>
       </c>
       <c r="L15" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B15,1),"),"," /* ",C15," - ",F15," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(1), /* 11 - PF_1 */</v>
       </c>
       <c r="M15" t="str">
-        <f>IF(ISBLANK(E15),CONCATENATE("NOT_ON_ADC", ", /* ", C15," - ",F15, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E15,LEN(E15)-1), ", /* ", C15," - ",F15, " */"))</f>
+        <f t="shared" si="5"/>
         <v>NOT_ON_ADC, /* 11 - PF_1 */</v>
       </c>
     </row>
     <row r="16" spans="2:13">
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="42">
         <v>12</v>
       </c>
       <c r="D16" t="s">
         <v>202</v>
       </c>
       <c r="F16" t="str">
-        <f>CONCATENATE(LEFT(B16,2),"_",RIGHT(B16,1))</f>
+        <f t="shared" si="0"/>
         <v>PF_0</v>
       </c>
       <c r="H16" t="str">
-        <f>CONCATENATE("static const uint8_t ",F16," = ", C16,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PF_0 = 12;</v>
       </c>
       <c r="J16" t="str">
-        <f>CONCATENATE(D16,", /* ", C16," - ",F16," */")</f>
+        <f t="shared" si="2"/>
         <v>T0A1, /* 12 - PF_0 */</v>
       </c>
       <c r="K16" t="str">
-        <f>CONCATENATE(LEFT(B16,2), ", /* ", C16," - ",F16, " */")</f>
+        <f t="shared" si="3"/>
         <v>PF, /* 12 - PF_0 */</v>
       </c>
       <c r="L16" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B16,1),"),"," /* ",C16," - ",F16," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(0), /* 12 - PF_0 */</v>
       </c>
       <c r="M16" t="str">
-        <f>IF(ISBLANK(E16),CONCATENATE("NOT_ON_ADC", ", /* ", C16," - ",F16, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E16,LEN(E16)-1), ", /* ", C16," - ",F16, " */"))</f>
+        <f t="shared" si="5"/>
         <v>NOT_ON_ADC, /* 12 - PF_0 */</v>
       </c>
     </row>
@@ -4080,27 +4116,27 @@
         <v>218</v>
       </c>
       <c r="F17" t="str">
-        <f>CONCATENATE(LEFT(B17,2),"_",RIGHT(B17,1))</f>
+        <f t="shared" si="0"/>
         <v>PF_2</v>
       </c>
       <c r="H17" t="str">
-        <f>CONCATENATE("static const uint8_t ",F17," = ", C17,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PF_2 = 13;</v>
       </c>
       <c r="J17" t="str">
-        <f>CONCATENATE(D17,", /* ", C17," - ",F17," */")</f>
+        <f t="shared" si="2"/>
         <v>T1A1, /* 13 - PF_2 */</v>
       </c>
       <c r="K17" t="str">
-        <f>CONCATENATE(LEFT(B17,2), ", /* ", C17," - ",F17, " */")</f>
+        <f t="shared" si="3"/>
         <v>PF, /* 13 - PF_2 */</v>
       </c>
       <c r="L17" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B17,1),"),"," /* ",C17," - ",F17," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(2), /* 13 - PF_2 */</v>
       </c>
       <c r="M17" t="str">
-        <f>IF(ISBLANK(E17),CONCATENATE("NOT_ON_ADC", ", /* ", C17," - ",F17, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E17,LEN(E17)-1), ", /* ", C17," - ",F17, " */"))</f>
+        <f t="shared" si="5"/>
         <v>NOT_ON_ADC, /* 13 - PF_2 */</v>
       </c>
     </row>
@@ -4115,27 +4151,27 @@
         <v>216</v>
       </c>
       <c r="F18" t="str">
-        <f>CONCATENATE(LEFT(B18,2),"_",RIGHT(B18,1))</f>
+        <f t="shared" si="0"/>
         <v>PB_3</v>
       </c>
       <c r="H18" t="str">
-        <f>CONCATENATE("static const uint8_t ",F18," = ", C18,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PB_3 = 14;</v>
       </c>
       <c r="J18" t="str">
-        <f>CONCATENATE(D18,", /* ", C18," - ",F18," */")</f>
+        <f t="shared" si="2"/>
         <v>T3B, /* 14 - PB_3 */</v>
       </c>
       <c r="K18" t="str">
-        <f>CONCATENATE(LEFT(B18,2), ", /* ", C18," - ",F18, " */")</f>
+        <f t="shared" si="3"/>
         <v>PB, /* 14 - PB_3 */</v>
       </c>
       <c r="L18" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B18,1),"),"," /* ",C18," - ",F18," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(3), /* 14 - PB_3 */</v>
       </c>
       <c r="M18" t="str">
-        <f>IF(ISBLANK(E18),CONCATENATE("NOT_ON_ADC", ", /* ", C18," - ",F18, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E18,LEN(E18)-1), ", /* ", C18," - ",F18, " */"))</f>
+        <f t="shared" si="5"/>
         <v>NOT_ON_ADC, /* 14 - PB_3 */</v>
       </c>
     </row>
@@ -4150,27 +4186,27 @@
         <v>203</v>
       </c>
       <c r="F19" t="str">
-        <f>CONCATENATE(LEFT(B19,2),"_",RIGHT(B19,1))</f>
+        <f t="shared" si="0"/>
         <v>PB_2</v>
       </c>
       <c r="H19" t="str">
-        <f>CONCATENATE("static const uint8_t ",F19," = ", C19,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PB_2 = 15;</v>
       </c>
       <c r="J19" t="str">
-        <f>CONCATENATE(D19,", /* ", C19," - ",F19," */")</f>
+        <f t="shared" si="2"/>
         <v>T3A, /* 15 - PB_2 */</v>
       </c>
       <c r="K19" t="str">
-        <f>CONCATENATE(LEFT(B19,2), ", /* ", C19," - ",F19, " */")</f>
+        <f t="shared" si="3"/>
         <v>PB, /* 15 - PB_2 */</v>
       </c>
       <c r="L19" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B19,1),"),"," /* ",C19," - ",F19," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(2), /* 15 - PB_2 */</v>
       </c>
       <c r="M19" t="str">
-        <f>IF(ISBLANK(E19),CONCATENATE("NOT_ON_ADC", ", /* ", C19," - ",F19, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E19,LEN(E19)-1), ", /* ", C19," - ",F19, " */"))</f>
+        <f t="shared" si="5"/>
         <v>NOT_ON_ADC, /* 15 - PB_2 */</v>
       </c>
     </row>
@@ -4188,31 +4224,31 @@
         <v>66</v>
       </c>
       <c r="F20" t="str">
-        <f>CONCATENATE(LEFT(B20,2),"_",RIGHT(B20,1))</f>
+        <f t="shared" si="0"/>
         <v>PE_3</v>
       </c>
       <c r="H20" t="str">
-        <f>CONCATENATE("static const uint8_t ",F20," = ", C20,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PE_3 = 16;</v>
       </c>
       <c r="I20" t="str">
-        <f>CONCATENATE("static const uint8_t ",E20," = ", C20,"; // ",F20)</f>
+        <f t="shared" ref="I20:I25" si="7">CONCATENATE("static const uint8_t ",E20," = ", C20,"; // ",F20)</f>
         <v>static const uint8_t A0 = 16; // PE_3</v>
       </c>
       <c r="J20" t="str">
-        <f>CONCATENATE(D20,", /* ", C20," - ",F20," */")</f>
+        <f t="shared" si="2"/>
         <v>NOT_ON_TIMER, /* 16 - PE_3 */</v>
       </c>
       <c r="K20" t="str">
-        <f>CONCATENATE(LEFT(B20,2), ", /* ", C20," - ",F20, " */")</f>
+        <f t="shared" si="3"/>
         <v>PE, /* 16 - PE_3 */</v>
       </c>
       <c r="L20" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B20,1),"),"," /* ",C20," - ",F20," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(3), /* 16 - PE_3 */</v>
       </c>
       <c r="M20" t="str">
-        <f>IF(ISBLANK(E20),CONCATENATE("NOT_ON_ADC", ", /* ", C20," - ",F20, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E20,LEN(E20)-1), ", /* ", C20," - ",F20, " */"))</f>
+        <f t="shared" si="5"/>
         <v>ADC_CTL_CH0, /* 16 - PE_3 */</v>
       </c>
     </row>
@@ -4230,31 +4266,31 @@
         <v>67</v>
       </c>
       <c r="F21" t="str">
-        <f>CONCATENATE(LEFT(B21,2),"_",RIGHT(B21,1))</f>
+        <f t="shared" si="0"/>
         <v>PE_2</v>
       </c>
       <c r="H21" t="str">
-        <f>CONCATENATE("static const uint8_t ",F21," = ", C21,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PE_2 = 17;</v>
       </c>
       <c r="I21" t="str">
-        <f>CONCATENATE("static const uint8_t ",E21," = ", C21,"; // ",F21)</f>
+        <f t="shared" si="7"/>
         <v>static const uint8_t A1 = 17; // PE_2</v>
       </c>
       <c r="J21" t="str">
-        <f>CONCATENATE(D21,", /* ", C21," - ",F21," */")</f>
+        <f t="shared" si="2"/>
         <v>NOT_ON_TIMER, /* 17 - PE_2 */</v>
       </c>
       <c r="K21" t="str">
-        <f>CONCATENATE(LEFT(B21,2), ", /* ", C21," - ",F21, " */")</f>
+        <f t="shared" si="3"/>
         <v>PE, /* 17 - PE_2 */</v>
       </c>
       <c r="L21" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B21,1),"),"," /* ",C21," - ",F21," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(2), /* 17 - PE_2 */</v>
       </c>
       <c r="M21" t="str">
-        <f>IF(ISBLANK(E21),CONCATENATE("NOT_ON_ADC", ", /* ", C21," - ",F21, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E21,LEN(E21)-1), ", /* ", C21," - ",F21, " */"))</f>
+        <f t="shared" si="5"/>
         <v>ADC_CTL_CH1, /* 17 - PE_2 */</v>
       </c>
     </row>
@@ -4272,31 +4308,31 @@
         <v>68</v>
       </c>
       <c r="F22" t="str">
-        <f>CONCATENATE(LEFT(B22,2),"_",RIGHT(B22,1))</f>
+        <f t="shared" si="0"/>
         <v>PE_1</v>
       </c>
       <c r="H22" t="str">
-        <f>CONCATENATE("static const uint8_t ",F22," = ", C22,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PE_1 = 18;</v>
       </c>
       <c r="I22" t="str">
-        <f>CONCATENATE("static const uint8_t ",E22," = ", C22,"; // ",F22)</f>
+        <f t="shared" si="7"/>
         <v>static const uint8_t A2 = 18; // PE_1</v>
       </c>
       <c r="J22" t="str">
-        <f>CONCATENATE(D22,", /* ", C22," - ",F22," */")</f>
+        <f t="shared" si="2"/>
         <v>NOT_ON_TIMER, /* 18 - PE_1 */</v>
       </c>
       <c r="K22" t="str">
-        <f>CONCATENATE(LEFT(B22,2), ", /* ", C22," - ",F22, " */")</f>
+        <f t="shared" si="3"/>
         <v>PE, /* 18 - PE_1 */</v>
       </c>
       <c r="L22" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B22,1),"),"," /* ",C22," - ",F22," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(1), /* 18 - PE_1 */</v>
       </c>
       <c r="M22" t="str">
-        <f>IF(ISBLANK(E22),CONCATENATE("NOT_ON_ADC", ", /* ", C22," - ",F22, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E22,LEN(E22)-1), ", /* ", C22," - ",F22, " */"))</f>
+        <f t="shared" si="5"/>
         <v>ADC_CTL_CH2, /* 18 - PE_1 */</v>
       </c>
     </row>
@@ -4314,31 +4350,31 @@
         <v>69</v>
       </c>
       <c r="F23" t="str">
-        <f>CONCATENATE(LEFT(B23,2),"_",RIGHT(B23,1))</f>
+        <f t="shared" si="0"/>
         <v>PE_0</v>
       </c>
       <c r="H23" t="str">
-        <f>CONCATENATE("static const uint8_t ",F23," = ", C23,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PE_0 = 19;</v>
       </c>
       <c r="I23" t="str">
-        <f>CONCATENATE("static const uint8_t ",E23," = ", C23,"; // ",F23)</f>
+        <f t="shared" si="7"/>
         <v>static const uint8_t A3 = 19; // PE_0</v>
       </c>
       <c r="J23" t="str">
-        <f>CONCATENATE(D23,", /* ", C23," - ",F23," */")</f>
+        <f t="shared" si="2"/>
         <v>NOT_ON_TIMER, /* 19 - PE_0 */</v>
       </c>
       <c r="K23" t="str">
-        <f>CONCATENATE(LEFT(B23,2), ", /* ", C23," - ",F23, " */")</f>
+        <f t="shared" si="3"/>
         <v>PE, /* 19 - PE_0 */</v>
       </c>
       <c r="L23" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B23,1),"),"," /* ",C23," - ",F23," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(0), /* 19 - PE_0 */</v>
       </c>
       <c r="M23" t="str">
-        <f>IF(ISBLANK(E23),CONCATENATE("NOT_ON_ADC", ", /* ", C23," - ",F23, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E23,LEN(E23)-1), ", /* ", C23," - ",F23, " */"))</f>
+        <f t="shared" si="5"/>
         <v>ADC_CTL_CH3, /* 19 - PE_0 */</v>
       </c>
     </row>
@@ -4356,31 +4392,31 @@
         <v>70</v>
       </c>
       <c r="F24" t="str">
-        <f>CONCATENATE(LEFT(B24,2),"_",RIGHT(B24,1))</f>
+        <f t="shared" si="0"/>
         <v>PD_3</v>
       </c>
       <c r="H24" t="str">
-        <f>CONCATENATE("static const uint8_t ",F24," = ", C24,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PD_3 = 20;</v>
       </c>
       <c r="I24" t="str">
-        <f>CONCATENATE("static const uint8_t ",E24," = ", C24,"; // ",F24)</f>
+        <f t="shared" si="7"/>
         <v>static const uint8_t A4 = 20; // PD_3</v>
       </c>
       <c r="J24" t="str">
-        <f>CONCATENATE(D24,", /* ", C24," - ",F24," */")</f>
+        <f t="shared" si="2"/>
         <v>WT3B, /* 20 - PD_3 */</v>
       </c>
       <c r="K24" t="str">
-        <f>CONCATENATE(LEFT(B24,2), ", /* ", C24," - ",F24, " */")</f>
+        <f t="shared" si="3"/>
         <v>PD, /* 20 - PD_3 */</v>
       </c>
       <c r="L24" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B24,1),"),"," /* ",C24," - ",F24," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(3), /* 20 - PD_3 */</v>
       </c>
       <c r="M24" t="str">
-        <f>IF(ISBLANK(E24),CONCATENATE("NOT_ON_ADC", ", /* ", C24," - ",F24, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E24,LEN(E24)-1), ", /* ", C24," - ",F24, " */"))</f>
+        <f t="shared" si="5"/>
         <v>ADC_CTL_CH4, /* 20 - PD_3 */</v>
       </c>
     </row>
@@ -4398,31 +4434,31 @@
         <v>71</v>
       </c>
       <c r="F25" t="str">
-        <f>CONCATENATE(LEFT(B25,2),"_",RIGHT(B25,1))</f>
+        <f t="shared" si="0"/>
         <v>PD_2</v>
       </c>
       <c r="H25" t="str">
-        <f>CONCATENATE("static const uint8_t ",F25," = ", C25,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PD_2 = 21;</v>
       </c>
       <c r="I25" t="str">
-        <f>CONCATENATE("static const uint8_t ",E25," = ", C25,"; // ",F25)</f>
+        <f t="shared" si="7"/>
         <v>static const uint8_t A5 = 21; // PD_2</v>
       </c>
       <c r="J25" t="str">
-        <f>CONCATENATE(D25,", /* ", C25," - ",F25," */")</f>
+        <f t="shared" si="2"/>
         <v>WT3A, /* 21 - PD_2 */</v>
       </c>
       <c r="K25" t="str">
-        <f>CONCATENATE(LEFT(B25,2), ", /* ", C25," - ",F25, " */")</f>
+        <f t="shared" si="3"/>
         <v>PD, /* 21 - PD_2 */</v>
       </c>
       <c r="L25" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B25,1),"),"," /* ",C25," - ",F25," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(2), /* 21 - PD_2 */</v>
       </c>
       <c r="M25" t="str">
-        <f>IF(ISBLANK(E25),CONCATENATE("NOT_ON_ADC", ", /* ", C25," - ",F25, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E25,LEN(E25)-1), ", /* ", C25," - ",F25, " */"))</f>
+        <f t="shared" si="5"/>
         <v>ADC_CTL_CH5, /* 21 - PD_2 */</v>
       </c>
     </row>
@@ -4437,27 +4473,27 @@
         <v>212</v>
       </c>
       <c r="F26" t="str">
-        <f>CONCATENATE(LEFT(B26,2),"_",RIGHT(B26,1))</f>
+        <f t="shared" si="0"/>
         <v>PC_7</v>
       </c>
       <c r="H26" t="str">
-        <f>CONCATENATE("static const uint8_t ",F26," = ", C26,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PC_7 = 22;</v>
       </c>
       <c r="J26" t="str">
-        <f>CONCATENATE(D26,", /* ", C26," - ",F26," */")</f>
+        <f t="shared" si="2"/>
         <v>WT1B, /* 22 - PC_7 */</v>
       </c>
       <c r="K26" t="str">
-        <f>CONCATENATE(LEFT(B26,2), ", /* ", C26," - ",F26, " */")</f>
+        <f t="shared" si="3"/>
         <v>PC, /* 22 - PC_7 */</v>
       </c>
       <c r="L26" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B26,1),"),"," /* ",C26," - ",F26," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(7), /* 22 - PC_7 */</v>
       </c>
       <c r="M26" t="str">
-        <f>IF(ISBLANK(E26),CONCATENATE("NOT_ON_ADC", ", /* ", C26," - ",F26, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E26,LEN(E26)-1), ", /* ", C26," - ",F26, " */"))</f>
+        <f t="shared" si="5"/>
         <v>NOT_ON_ADC, /* 22 - PC_7 */</v>
       </c>
     </row>
@@ -4472,27 +4508,27 @@
         <v>213</v>
       </c>
       <c r="F27" t="str">
-        <f>CONCATENATE(LEFT(B27,2),"_",RIGHT(B27,1))</f>
+        <f t="shared" si="0"/>
         <v>PC_6</v>
       </c>
       <c r="H27" t="str">
-        <f>CONCATENATE("static const uint8_t ",F27," = ", C27,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PC_6 = 23;</v>
       </c>
       <c r="J27" t="str">
-        <f>CONCATENATE(D27,", /* ", C27," - ",F27," */")</f>
+        <f t="shared" si="2"/>
         <v>WT1A, /* 23 - PC_6 */</v>
       </c>
       <c r="K27" t="str">
-        <f>CONCATENATE(LEFT(B27,2), ", /* ", C27," - ",F27, " */")</f>
+        <f t="shared" si="3"/>
         <v>PC, /* 23 - PC_6 */</v>
       </c>
       <c r="L27" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B27,1),"),"," /* ",C27," - ",F27," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(6), /* 23 - PC_6 */</v>
       </c>
       <c r="M27" t="str">
-        <f>IF(ISBLANK(E27),CONCATENATE("NOT_ON_ADC", ", /* ", C27," - ",F27, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E27,LEN(E27)-1), ", /* ", C27," - ",F27, " */"))</f>
+        <f t="shared" si="5"/>
         <v>NOT_ON_ADC, /* 23 - PC_6 */</v>
       </c>
     </row>
@@ -4507,27 +4543,27 @@
         <v>214</v>
       </c>
       <c r="F28" t="str">
-        <f>CONCATENATE(LEFT(B28,2),"_",RIGHT(B28,1))</f>
+        <f t="shared" si="0"/>
         <v>PC_5</v>
       </c>
       <c r="H28" t="str">
-        <f>CONCATENATE("static const uint8_t ",F28," = ", C28,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PC_5 = 24;</v>
       </c>
       <c r="J28" t="str">
-        <f>CONCATENATE(D28,", /* ", C28," - ",F28," */")</f>
+        <f t="shared" si="2"/>
         <v>WT0B, /* 24 - PC_5 */</v>
       </c>
       <c r="K28" t="str">
-        <f>CONCATENATE(LEFT(B28,2), ", /* ", C28," - ",F28, " */")</f>
+        <f t="shared" si="3"/>
         <v>PC, /* 24 - PC_5 */</v>
       </c>
       <c r="L28" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B28,1),"),"," /* ",C28," - ",F28," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(5), /* 24 - PC_5 */</v>
       </c>
       <c r="M28" t="str">
-        <f>IF(ISBLANK(E28),CONCATENATE("NOT_ON_ADC", ", /* ", C28," - ",F28, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E28,LEN(E28)-1), ", /* ", C28," - ",F28, " */"))</f>
+        <f t="shared" si="5"/>
         <v>NOT_ON_ADC, /* 24 - PC_5 */</v>
       </c>
     </row>
@@ -4542,27 +4578,27 @@
         <v>215</v>
       </c>
       <c r="F29" t="str">
-        <f>CONCATENATE(LEFT(B29,2),"_",RIGHT(B29,1))</f>
+        <f t="shared" si="0"/>
         <v>PC_4</v>
       </c>
       <c r="H29" t="str">
-        <f>CONCATENATE("static const uint8_t ",F29," = ", C29,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PC_4 = 25;</v>
       </c>
       <c r="J29" t="str">
-        <f>CONCATENATE(D29,", /* ", C29," - ",F29," */")</f>
+        <f t="shared" si="2"/>
         <v>WT0A, /* 25 - PC_4 */</v>
       </c>
       <c r="K29" t="str">
-        <f>CONCATENATE(LEFT(B29,2), ", /* ", C29," - ",F29, " */")</f>
+        <f t="shared" si="3"/>
         <v>PC, /* 25 - PC_4 */</v>
       </c>
       <c r="L29" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B29,1),"),"," /* ",C29," - ",F29," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(4), /* 25 - PC_4 */</v>
       </c>
       <c r="M29" t="str">
-        <f>IF(ISBLANK(E29),CONCATENATE("NOT_ON_ADC", ", /* ", C29," - ",F29, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E29,LEN(E29)-1), ", /* ", C29," - ",F29, " */"))</f>
+        <f t="shared" si="5"/>
         <v>NOT_ON_ADC, /* 25 - PC_4 */</v>
       </c>
     </row>
@@ -4577,27 +4613,27 @@
         <v>198</v>
       </c>
       <c r="F30" t="str">
-        <f>CONCATENATE(LEFT(B30,2),"_",RIGHT(B30,1))</f>
+        <f t="shared" si="0"/>
         <v>PA_2</v>
       </c>
       <c r="H30" t="str">
-        <f>CONCATENATE("static const uint8_t ",F30," = ", C30,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PA_2 = 26;</v>
       </c>
       <c r="J30" t="str">
-        <f>CONCATENATE(D30,", /* ", C30," - ",F30," */")</f>
+        <f t="shared" si="2"/>
         <v>NOT_ON_TIMER, /* 26 - PA_2 */</v>
       </c>
       <c r="K30" t="str">
-        <f>CONCATENATE(LEFT(B30,2), ", /* ", C30," - ",F30, " */")</f>
+        <f t="shared" si="3"/>
         <v>PA, /* 26 - PA_2 */</v>
       </c>
       <c r="L30" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B30,1),"),"," /* ",C30," - ",F30," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(2), /* 26 - PA_2 */</v>
       </c>
       <c r="M30" t="str">
-        <f>IF(ISBLANK(E30),CONCATENATE("NOT_ON_ADC", ", /* ", C30," - ",F30, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E30,LEN(E30)-1), ", /* ", C30," - ",F30, " */"))</f>
+        <f t="shared" si="5"/>
         <v>NOT_ON_ADC, /* 26 - PA_2 */</v>
       </c>
     </row>
@@ -4612,27 +4648,27 @@
         <v>198</v>
       </c>
       <c r="F31" t="str">
-        <f>CONCATENATE(LEFT(B31,2),"_",RIGHT(B31,1))</f>
+        <f t="shared" si="0"/>
         <v>PA_3</v>
       </c>
       <c r="H31" t="str">
-        <f>CONCATENATE("static const uint8_t ",F31," = ", C31,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PA_3 = 27;</v>
       </c>
       <c r="J31" t="str">
-        <f>CONCATENATE(D31,", /* ", C31," - ",F31," */")</f>
+        <f t="shared" si="2"/>
         <v>NOT_ON_TIMER, /* 27 - PA_3 */</v>
       </c>
       <c r="K31" t="str">
-        <f>CONCATENATE(LEFT(B31,2), ", /* ", C31," - ",F31, " */")</f>
+        <f t="shared" si="3"/>
         <v>PA, /* 27 - PA_3 */</v>
       </c>
       <c r="L31" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B31,1),"),"," /* ",C31," - ",F31," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(3), /* 27 - PA_3 */</v>
       </c>
       <c r="M31" t="str">
-        <f>IF(ISBLANK(E31),CONCATENATE("NOT_ON_ADC", ", /* ", C31," - ",F31, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E31,LEN(E31)-1), ", /* ", C31," - ",F31, " */"))</f>
+        <f t="shared" si="5"/>
         <v>NOT_ON_ADC, /* 27 - PA_3 */</v>
       </c>
     </row>
@@ -4647,27 +4683,27 @@
         <v>198</v>
       </c>
       <c r="F32" t="str">
-        <f>CONCATENATE(LEFT(B32,2),"_",RIGHT(B32,1))</f>
+        <f t="shared" si="0"/>
         <v>PA_4</v>
       </c>
       <c r="H32" t="str">
-        <f>CONCATENATE("static const uint8_t ",F32," = ", C32,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PA_4 = 28;</v>
       </c>
       <c r="J32" t="str">
-        <f>CONCATENATE(D32,", /* ", C32," - ",F32," */")</f>
+        <f t="shared" si="2"/>
         <v>NOT_ON_TIMER, /* 28 - PA_4 */</v>
       </c>
       <c r="K32" t="str">
-        <f>CONCATENATE(LEFT(B32,2), ", /* ", C32," - ",F32, " */")</f>
+        <f t="shared" si="3"/>
         <v>PA, /* 28 - PA_4 */</v>
       </c>
       <c r="L32" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B32,1),"),"," /* ",C32," - ",F32," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(4), /* 28 - PA_4 */</v>
       </c>
       <c r="M32" t="str">
-        <f>IF(ISBLANK(E32),CONCATENATE("NOT_ON_ADC", ", /* ", C32," - ",F32, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E32,LEN(E32)-1), ", /* ", C32," - ",F32, " */"))</f>
+        <f t="shared" si="5"/>
         <v>NOT_ON_ADC, /* 28 - PA_4 */</v>
       </c>
     </row>
@@ -4682,27 +4718,27 @@
         <v>198</v>
       </c>
       <c r="F33" t="str">
-        <f>CONCATENATE(LEFT(B33,2),"_",RIGHT(B33,1))</f>
+        <f t="shared" si="0"/>
         <v>PA_5</v>
       </c>
       <c r="H33" t="str">
-        <f>CONCATENATE("static const uint8_t ",F33," = ", C33,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PA_5 = 29;</v>
       </c>
       <c r="J33" t="str">
-        <f>CONCATENATE(D33,", /* ", C33," - ",F33," */")</f>
+        <f t="shared" si="2"/>
         <v>NOT_ON_TIMER, /* 29 - PA_5 */</v>
       </c>
       <c r="K33" t="str">
-        <f>CONCATENATE(LEFT(B33,2), ", /* ", C33," - ",F33, " */")</f>
+        <f t="shared" si="3"/>
         <v>PA, /* 29 - PA_5 */</v>
       </c>
       <c r="L33" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B33,1),"),"," /* ",C33," - ",F33," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(5), /* 29 - PA_5 */</v>
       </c>
       <c r="M33" t="str">
-        <f>IF(ISBLANK(E33),CONCATENATE("NOT_ON_ADC", ", /* ", C33," - ",F33, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E33,LEN(E33)-1), ", /* ", C33," - ",F33, " */"))</f>
+        <f t="shared" si="5"/>
         <v>NOT_ON_ADC, /* 29 - PA_5 */</v>
       </c>
     </row>
@@ -4717,27 +4753,27 @@
         <v>196</v>
       </c>
       <c r="F34" t="str">
-        <f>CONCATENATE(LEFT(B34,2),"_",RIGHT(B34,1))</f>
+        <f t="shared" si="0"/>
         <v>PB_0</v>
       </c>
       <c r="H34" t="str">
-        <f>CONCATENATE("static const uint8_t ",F34," = ", C34,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PB_0 = 30;</v>
       </c>
       <c r="J34" t="str">
-        <f>CONCATENATE(D34,", /* ", C34," - ",F34," */")</f>
+        <f t="shared" si="2"/>
         <v>T2A0, /* 30 - PB_0 */</v>
       </c>
       <c r="K34" t="str">
-        <f>CONCATENATE(LEFT(B34,2), ", /* ", C34," - ",F34, " */")</f>
+        <f t="shared" si="3"/>
         <v>PB, /* 30 - PB_0 */</v>
       </c>
       <c r="L34" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B34,1),"),"," /* ",C34," - ",F34," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(0), /* 30 - PB_0 */</v>
       </c>
       <c r="M34" t="str">
-        <f>IF(ISBLANK(E34),CONCATENATE("NOT_ON_ADC", ", /* ", C34," - ",F34, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E34,LEN(E34)-1), ", /* ", C34," - ",F34, " */"))</f>
+        <f t="shared" si="5"/>
         <v>NOT_ON_ADC, /* 30 - PB_0 */</v>
       </c>
     </row>
@@ -4752,27 +4788,27 @@
         <v>197</v>
       </c>
       <c r="F35" t="str">
-        <f>CONCATENATE(LEFT(B35,2),"_",RIGHT(B35,1))</f>
+        <f t="shared" si="0"/>
         <v>PB_1</v>
       </c>
       <c r="H35" t="str">
-        <f>CONCATENATE("static const uint8_t ",F35," = ", C35,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PB_1 = 31;</v>
       </c>
       <c r="J35" t="str">
-        <f>CONCATENATE(D35,", /* ", C35," - ",F35," */")</f>
+        <f t="shared" si="2"/>
         <v>T2B, /* 31 - PB_1 */</v>
       </c>
       <c r="K35" t="str">
-        <f>CONCATENATE(LEFT(B35,2), ", /* ", C35," - ",F35, " */")</f>
+        <f t="shared" si="3"/>
         <v>PB, /* 31 - PB_1 */</v>
       </c>
       <c r="L35" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B35,1),"),"," /* ",C35," - ",F35," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(1), /* 31 - PB_1 */</v>
       </c>
       <c r="M35" t="str">
-        <f>IF(ISBLANK(E35),CONCATENATE("NOT_ON_ADC", ", /* ", C35," - ",F35, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E35,LEN(E35)-1), ", /* ", C35," - ",F35, " */"))</f>
+        <f t="shared" si="5"/>
         <v>NOT_ON_ADC, /* 31 - PB_1 */</v>
       </c>
     </row>
@@ -4787,62 +4823,62 @@
         <v>211</v>
       </c>
       <c r="F36" t="str">
-        <f>CONCATENATE(LEFT(B36,2),"_",RIGHT(B36,1))</f>
+        <f t="shared" si="0"/>
         <v>PD_6</v>
       </c>
       <c r="H36" t="str">
-        <f>CONCATENATE("static const uint8_t ",F36," = ", C36,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PD_6 = 32;</v>
       </c>
       <c r="J36" t="str">
-        <f>CONCATENATE(D36,", /* ", C36," - ",F36," */")</f>
+        <f t="shared" si="2"/>
         <v>WT5A, /* 32 - PD_6 */</v>
       </c>
       <c r="K36" t="str">
-        <f>CONCATENATE(LEFT(B36,2), ", /* ", C36," - ",F36, " */")</f>
+        <f t="shared" si="3"/>
         <v>PD, /* 32 - PD_6 */</v>
       </c>
       <c r="L36" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B36,1),"),"," /* ",C36," - ",F36," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(6), /* 32 - PD_6 */</v>
       </c>
       <c r="M36" t="str">
-        <f>IF(ISBLANK(E36),CONCATENATE("NOT_ON_ADC", ", /* ", C36," - ",F36, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E36,LEN(E36)-1), ", /* ", C36," - ",F36, " */"))</f>
+        <f t="shared" si="5"/>
         <v>NOT_ON_ADC, /* 32 - PD_6 */</v>
       </c>
     </row>
     <row r="37" spans="2:13">
-      <c r="B37" s="12" t="s">
+      <c r="B37" s="51" t="s">
         <v>107</v>
       </c>
-      <c r="C37" s="10">
+      <c r="C37" s="42">
         <v>33</v>
       </c>
       <c r="D37" t="s">
         <v>210</v>
       </c>
       <c r="F37" t="str">
-        <f>CONCATENATE(LEFT(B37,2),"_",RIGHT(B37,1))</f>
+        <f t="shared" si="0"/>
         <v>PD_7</v>
       </c>
       <c r="H37" t="str">
-        <f>CONCATENATE("static const uint8_t ",F37," = ", C37,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PD_7 = 33;</v>
       </c>
       <c r="J37" t="str">
-        <f>CONCATENATE(D37,", /* ", C37," - ",F37," */")</f>
+        <f t="shared" si="2"/>
         <v>WT5B, /* 33 - PD_7 */</v>
       </c>
       <c r="K37" t="str">
-        <f>CONCATENATE(LEFT(B37,2), ", /* ", C37," - ",F37, " */")</f>
+        <f t="shared" si="3"/>
         <v>PD, /* 33 - PD_7 */</v>
       </c>
       <c r="L37" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B37,1),"),"," /* ",C37," - ",F37," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(7), /* 33 - PD_7 */</v>
       </c>
       <c r="M37" t="str">
-        <f>IF(ISBLANK(E37),CONCATENATE("NOT_ON_ADC", ", /* ", C37," - ",F37, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E37,LEN(E37)-1), ", /* ", C37," - ",F37, " */"))</f>
+        <f t="shared" si="5"/>
         <v>NOT_ON_ADC, /* 33 - PD_7 */</v>
       </c>
     </row>
@@ -4857,27 +4893,27 @@
         <v>209</v>
       </c>
       <c r="F38" t="str">
-        <f>CONCATENATE(LEFT(B38,2),"_",RIGHT(B38,1))</f>
+        <f t="shared" si="0"/>
         <v>PF_4</v>
       </c>
       <c r="H38" t="str">
-        <f>CONCATENATE("static const uint8_t ",F38," = ", C38,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PF_4 = 34;</v>
       </c>
       <c r="J38" t="str">
-        <f>CONCATENATE(D38,", /* ", C38," - ",F38," */")</f>
+        <f t="shared" si="2"/>
         <v>T2A1, /* 34 - PF_4 */</v>
       </c>
       <c r="K38" t="str">
-        <f>CONCATENATE(LEFT(B38,2), ", /* ", C38," - ",F38, " */")</f>
+        <f t="shared" si="3"/>
         <v>PF, /* 34 - PF_4 */</v>
       </c>
       <c r="L38" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B38,1),"),"," /* ",C38," - ",F38," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(4), /* 34 - PF_4 */</v>
       </c>
       <c r="M38" t="str">
-        <f>IF(ISBLANK(E38),CONCATENATE("NOT_ON_ADC", ", /* ", C38," - ",F38, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E38,LEN(E38)-1), ", /* ", C38," - ",F38, " */"))</f>
+        <f t="shared" si="5"/>
         <v>NOT_ON_ADC, /* 34 - PF_4 */</v>
       </c>
     </row>
@@ -4892,27 +4928,27 @@
         <v>200</v>
       </c>
       <c r="F39" t="str">
-        <f>CONCATENATE(LEFT(B39,2),"_",RIGHT(B39,1))</f>
+        <f t="shared" si="0"/>
         <v>PB_6</v>
       </c>
       <c r="H39" t="str">
-        <f>CONCATENATE("static const uint8_t ",F39," = ", C39,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PB_6 = 35;</v>
       </c>
       <c r="J39" t="str">
-        <f>CONCATENATE(D39,", /* ", C39," - ",F39," */")</f>
+        <f t="shared" si="2"/>
         <v>T0A0, /* 35 - PB_6 */</v>
       </c>
       <c r="K39" t="str">
-        <f>CONCATENATE(LEFT(B39,2), ", /* ", C39," - ",F39, " */")</f>
+        <f t="shared" si="3"/>
         <v>PB, /* 35 - PB_6 */</v>
       </c>
       <c r="L39" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B39,1),"),"," /* ",C39," - ",F39," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(6), /* 35 - PB_6 */</v>
       </c>
       <c r="M39" t="str">
-        <f>IF(ISBLANK(E39),CONCATENATE("NOT_ON_ADC", ", /* ", C39," - ",F39, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E39,LEN(E39)-1), ", /* ", C39," - ",F39, " */"))</f>
+        <f t="shared" si="5"/>
         <v>NOT_ON_ADC, /* 35 - PB_6 */</v>
       </c>
     </row>
@@ -4927,27 +4963,27 @@
         <v>201</v>
       </c>
       <c r="F40" t="str">
-        <f>CONCATENATE(LEFT(B40,2),"_",RIGHT(B40,1))</f>
+        <f t="shared" si="0"/>
         <v>PB_7</v>
       </c>
       <c r="H40" t="str">
-        <f>CONCATENATE("static const uint8_t ",F40," = ", C40,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t PB_7 = 36;</v>
       </c>
       <c r="J40" t="str">
-        <f>CONCATENATE(D40,", /* ", C40," - ",F40," */")</f>
+        <f t="shared" si="2"/>
         <v>T0B0, /* 36 - PB_7 */</v>
       </c>
       <c r="K40" t="str">
-        <f>CONCATENATE(LEFT(B40,2), ", /* ", C40," - ",F40, " */")</f>
+        <f t="shared" si="3"/>
         <v>PB, /* 36 - PB_7 */</v>
       </c>
       <c r="L40" t="str">
-        <f>CONCATENATE("BV(",RIGHT(B40,1),"),"," /* ",C40," - ",F40," */")</f>
+        <f t="shared" si="4"/>
         <v>BV(7), /* 36 - PB_7 */</v>
       </c>
       <c r="M40" t="str">
-        <f>IF(ISBLANK(E40),CONCATENATE("NOT_ON_ADC", ", /* ", C40," - ",F40, " */"),CONCATENATE("ADC_CTL_CH",RIGHT(E40,LEN(E40)-1), ", /* ", C40," - ",F40, " */"))</f>
+        <f t="shared" si="5"/>
         <v>NOT_ON_ADC, /* 36 - PB_7 */</v>
       </c>
     </row>
@@ -4959,7 +4995,7 @@
         <v>37</v>
       </c>
       <c r="H41" t="str">
-        <f>CONCATENATE("static const uint8_t ",F41," = ", C41,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t  = 37;</v>
       </c>
       <c r="J41" s="17" t="s">
@@ -4983,7 +5019,7 @@
         <v>38</v>
       </c>
       <c r="H42" t="str">
-        <f>CONCATENATE("static const uint8_t ",F42," = ", C42,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t  = 38;</v>
       </c>
       <c r="J42" s="17" t="s">
@@ -5007,7 +5043,7 @@
         <v>39</v>
       </c>
       <c r="H43" t="str">
-        <f>CONCATENATE("static const uint8_t ",F43," = ", C43,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t  = 39;</v>
       </c>
       <c r="J43" s="17" t="s">
@@ -5031,7 +5067,7 @@
         <v>40</v>
       </c>
       <c r="H44" t="str">
-        <f>CONCATENATE("static const uint8_t ",F44," = ", C44,";")</f>
+        <f t="shared" si="1"/>
         <v>static const uint8_t  = 40;</v>
       </c>
       <c r="J44" s="17" t="s">
@@ -5047,7 +5083,320 @@
         <v>236</v>
       </c>
     </row>
+    <row r="50" spans="2:3">
+      <c r="C50" s="43" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3">
+      <c r="B51" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3">
+      <c r="B52" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3">
+      <c r="B53" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3">
+      <c r="B54" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54" s="22">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3">
+      <c r="B55" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55" s="22">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3">
+      <c r="B56" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56" s="22">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3">
+      <c r="B57" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57" s="22">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3">
+      <c r="B58" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C58" s="22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3">
+      <c r="B59" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C59" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3">
+      <c r="B60" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="C60" s="22">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3">
+      <c r="B61" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="C61" s="22">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3">
+      <c r="B62" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C62" s="41">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3">
+      <c r="B63" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="C63" s="41">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3">
+      <c r="B64" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C64" s="22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3">
+      <c r="B65" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C65" s="22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3">
+      <c r="B66" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C66" s="22">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3">
+      <c r="B67" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C67" s="22">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3">
+      <c r="B68" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="C68" s="22">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3">
+      <c r="B69" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="C69" s="22">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3">
+      <c r="B70" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="C70" s="22">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3">
+      <c r="B71" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="C71" s="22">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3">
+      <c r="B72" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C72" s="22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3">
+      <c r="B73" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C73" s="22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3">
+      <c r="B74" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C74" s="41">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3">
+      <c r="B75" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C75" s="41">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3">
+      <c r="B76" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C76" s="22">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3">
+      <c r="B77" s="51" t="s">
+        <v>107</v>
+      </c>
+      <c r="C77" s="42">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3">
+      <c r="B78" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C78" s="22">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3">
+      <c r="B79" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C79" s="22">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3">
+      <c r="B80" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="C80" s="22">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3">
+      <c r="B81" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="C81" s="22">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3">
+      <c r="B82" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C82" s="22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3">
+      <c r="B83" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C83" s="22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3">
+      <c r="B84" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="C84" s="42">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3">
+      <c r="B85" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C85" s="22">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3">
+      <c r="B86" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C86" s="22">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3">
+      <c r="B87" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C87" s="22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3">
+      <c r="B88" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C88" s="22">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="B52:C88">
+    <sortCondition ref="B52"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Recent modifications to layout. Switching to resistor arrays. Adding Roadrunner image.
</commit_message>
<xml_diff>
--- a/PinMap.xlsx
+++ b/PinMap.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="11475" windowHeight="4950" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="11475" windowHeight="4950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1040,6 +1040,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1059,9 +1062,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1983,12 +1983,12 @@
       <c r="F37" s="4"/>
     </row>
     <row r="39" spans="4:7">
-      <c r="D39" s="44" t="s">
+      <c r="D39" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="E39" s="44"/>
-      <c r="F39" s="44"/>
-      <c r="G39" s="44"/>
+      <c r="E39" s="45"/>
+      <c r="F39" s="45"/>
+      <c r="G39" s="45"/>
     </row>
     <row r="40" spans="4:7">
       <c r="D40" t="s">
@@ -2493,8 +2493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U44"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="40" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="U43" sqref="U43"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="40" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2529,22 +2529,22 @@
       </c>
     </row>
     <row r="3" spans="1:21">
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="49" t="s">
         <v>120</v>
       </c>
-      <c r="D3" s="48"/>
+      <c r="D3" s="49"/>
     </row>
     <row r="4" spans="1:21">
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="50" t="s">
         <v>119</v>
       </c>
-      <c r="D4" s="49"/>
+      <c r="D4" s="50"/>
     </row>
     <row r="5" spans="1:21">
-      <c r="C5" s="50" t="s">
+      <c r="C5" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="D5" s="50"/>
+      <c r="D5" s="51"/>
     </row>
     <row r="6" spans="1:21">
       <c r="L6" s="19" t="s">
@@ -3342,7 +3342,7 @@
       </c>
     </row>
     <row r="36" spans="1:21">
-      <c r="J36" s="45" t="s">
+      <c r="J36" s="46" t="s">
         <v>188</v>
       </c>
       <c r="K36" s="28"/>
@@ -3364,7 +3364,7 @@
       <c r="U36" s="28"/>
     </row>
     <row r="37" spans="1:21">
-      <c r="J37" s="46"/>
+      <c r="J37" s="47"/>
       <c r="K37" s="7"/>
       <c r="L37" s="24" t="s">
         <v>58</v>
@@ -3384,7 +3384,7 @@
       <c r="U37" s="7"/>
     </row>
     <row r="38" spans="1:21">
-      <c r="J38" s="46"/>
+      <c r="J38" s="47"/>
       <c r="K38" s="7"/>
       <c r="L38" s="24" t="s">
         <v>59</v>
@@ -3404,7 +3404,7 @@
       <c r="U38" s="7"/>
     </row>
     <row r="39" spans="1:21">
-      <c r="J39" s="47"/>
+      <c r="J39" s="48"/>
       <c r="K39" s="5"/>
       <c r="L39" s="26" t="s">
         <v>60</v>
@@ -3424,7 +3424,7 @@
       <c r="U39" s="5"/>
     </row>
     <row r="40" spans="1:21">
-      <c r="J40" s="45" t="s">
+      <c r="J40" s="46" t="s">
         <v>187</v>
       </c>
       <c r="K40" s="28" t="s">
@@ -3450,7 +3450,7 @@
       </c>
     </row>
     <row r="41" spans="1:21">
-      <c r="J41" s="46"/>
+      <c r="J41" s="47"/>
       <c r="K41" s="7" t="s">
         <v>169</v>
       </c>
@@ -3474,7 +3474,7 @@
       </c>
     </row>
     <row r="42" spans="1:21">
-      <c r="J42" s="46"/>
+      <c r="J42" s="47"/>
       <c r="K42" s="7" t="s">
         <v>167</v>
       </c>
@@ -3496,7 +3496,7 @@
       <c r="U42" s="7"/>
     </row>
     <row r="43" spans="1:21">
-      <c r="J43" s="47"/>
+      <c r="J43" s="48"/>
       <c r="K43" s="5" t="s">
         <v>170</v>
       </c>
@@ -3558,7 +3558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:M88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
@@ -4071,7 +4071,7 @@
       </c>
     </row>
     <row r="16" spans="2:13">
-      <c r="B16" s="51" t="s">
+      <c r="B16" s="44" t="s">
         <v>33</v>
       </c>
       <c r="C16" s="42">
@@ -4848,7 +4848,7 @@
       </c>
     </row>
     <row r="37" spans="2:13">
-      <c r="B37" s="51" t="s">
+      <c r="B37" s="44" t="s">
         <v>107</v>
       </c>
       <c r="C37" s="42">
@@ -5297,7 +5297,7 @@
       </c>
     </row>
     <row r="77" spans="2:3">
-      <c r="B77" s="51" t="s">
+      <c r="B77" s="44" t="s">
         <v>107</v>
       </c>
       <c r="C77" s="42">
@@ -5353,7 +5353,7 @@
       </c>
     </row>
     <row r="84" spans="2:3">
-      <c r="B84" s="51" t="s">
+      <c r="B84" s="44" t="s">
         <v>33</v>
       </c>
       <c r="C84" s="42">

</xml_diff>